<commit_message>
Adicionado mais itens na estimativa
</commit_message>
<xml_diff>
--- a/artefatos/ESTIMATIVA.xlsx
+++ b/artefatos/ESTIMATIVA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Laboratorio de Engenharia\Segunda tentativa\ToCBooks\artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA861149-809C-4298-A8C8-DB9F76E82C34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F3B9CC-688A-4724-9064-BB13A39E6A8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D9FF7230-91BA-A544-8A5A-3054F2DD43A9}"/>
+    <workbookView xWindow="4390" yWindow="2540" windowWidth="29700" windowHeight="14020" xr2:uid="{D9FF7230-91BA-A544-8A5A-3054F2DD43A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>(horas)</t>
   </si>
@@ -87,6 +87,87 @@
   </si>
   <si>
     <t>Implementar as interfaces e escrever as classes principais</t>
+  </si>
+  <si>
+    <t>Criar o login e signup</t>
+  </si>
+  <si>
+    <t>Criar o primeiro mapa das entidade do banco</t>
+  </si>
+  <si>
+    <t>Criar classes de validações obrigatórias de Cliente</t>
+  </si>
+  <si>
+    <t>Criar classes de validações obrigatórias de Livro</t>
+  </si>
+  <si>
+    <t>Criar classes da lógica do estoque</t>
+  </si>
+  <si>
+    <t>Criar carrinho de compra</t>
+  </si>
+  <si>
+    <t>Criar as validações do carrinho</t>
+  </si>
+  <si>
+    <t>Criar a classe de compra</t>
+  </si>
+  <si>
+    <t>Criar os validadores de compra</t>
+  </si>
+  <si>
+    <t>Criar a lógica de compra</t>
+  </si>
+  <si>
+    <t>Criar a tela de compra</t>
+  </si>
+  <si>
+    <t>Criar a tela de devolução</t>
+  </si>
+  <si>
+    <t>Criar a lógica de devolução</t>
+  </si>
+  <si>
+    <t>Criar a lógica do cupom de desconto</t>
+  </si>
+  <si>
+    <t>Adicionar a tela o cupom de desconto</t>
+  </si>
+  <si>
+    <t>Criar o Read de Cliente</t>
+  </si>
+  <si>
+    <t>Criar o Inativar de Cliente</t>
+  </si>
+  <si>
+    <t>Criar o Update de Cliente</t>
+  </si>
+  <si>
+    <t>Criar o Create de Cliente</t>
+  </si>
+  <si>
+    <t>Criar o Create de Livro</t>
+  </si>
+  <si>
+    <t>Criar o Read de Livro</t>
+  </si>
+  <si>
+    <t>Criar o Inativar de Livro</t>
+  </si>
+  <si>
+    <t>Ciar o modelo que representa o Cliente</t>
+  </si>
+  <si>
+    <t>Criaro modelo que representa o Livro</t>
+  </si>
+  <si>
+    <t>Criar o modelo que representa o Estoque</t>
+  </si>
+  <si>
+    <t>Criar o Update de Livro</t>
+  </si>
+  <si>
+    <t>Criar classe de modelo que represente o Cartão de Crédito</t>
   </si>
 </sst>
 </file>
@@ -243,9 +324,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -282,11 +360,464 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="69">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -843,10 +1374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B692412-8401-4F44-8DDD-33476696CC96}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -896,11 +1427,11 @@
       <c r="E2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="I2" s="6" t="s">
         <v>9</v>
       </c>
@@ -919,633 +1450,1054 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+      <c r="A4" s="25">
         <v>1</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>2</v>
       </c>
-      <c r="D4" s="16">
-        <v>3</v>
-      </c>
-      <c r="E4" s="16">
+      <c r="D4" s="15">
+        <v>3</v>
+      </c>
+      <c r="E4" s="15">
         <v>7</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="16"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="26">
+      <c r="A5" s="25">
         <v>2</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>4</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <v>6</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="15">
         <v>10</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="15"/>
+      <c r="G5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="16"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="26">
-        <v>3</v>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="25">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="16">
-        <v>3</v>
-      </c>
-      <c r="D6" s="16">
+      <c r="C6" s="15">
+        <v>3</v>
+      </c>
+      <c r="D6" s="15">
         <v>4</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>6</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16" t="s">
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="26">
+      <c r="A7" s="25">
         <v>4</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>5</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <v>7</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="15">
         <v>10</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16" t="s">
+      <c r="F7" s="15"/>
+      <c r="G7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="26">
+      <c r="A8" s="25">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="B8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="15">
+        <v>4</v>
+      </c>
+      <c r="D8" s="15">
+        <v>7</v>
+      </c>
+      <c r="E8" s="15">
+        <v>9</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="26">
+      <c r="A9" s="25">
         <v>6</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
+      <c r="B9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="15">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15">
+        <v>3</v>
+      </c>
+      <c r="E9" s="15">
+        <v>4</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="26">
+      <c r="A10" s="25">
         <v>7</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="B10" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="15">
+        <v>2</v>
+      </c>
+      <c r="D10" s="15">
+        <v>3</v>
+      </c>
+      <c r="E10" s="15">
+        <v>4</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="26">
+      <c r="A11" s="25">
         <v>8</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
+      <c r="B11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="15">
+        <v>6</v>
+      </c>
+      <c r="D11" s="15">
+        <v>9</v>
+      </c>
+      <c r="E11" s="15">
+        <v>11</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="26">
+      <c r="A12" s="25">
         <v>9</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="B12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="15">
+        <v>2</v>
+      </c>
+      <c r="D12" s="15">
+        <v>3</v>
+      </c>
+      <c r="E12" s="15">
+        <v>4</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="26">
+      <c r="A13" s="25">
         <v>10</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
+      <c r="B13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="15">
+        <v>1</v>
+      </c>
+      <c r="D13" s="15">
+        <v>3</v>
+      </c>
+      <c r="E13" s="15">
+        <v>4</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="26">
+      <c r="A14" s="25">
         <v>11</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="B14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="15">
+        <v>2</v>
+      </c>
+      <c r="D14" s="15">
+        <v>3</v>
+      </c>
+      <c r="E14" s="15">
+        <v>5</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="26">
+      <c r="A15" s="25">
         <v>12</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
+      <c r="B15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="15">
+        <v>5</v>
+      </c>
+      <c r="D15" s="15">
+        <v>7</v>
+      </c>
+      <c r="E15" s="15">
+        <v>8</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="26"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+      <c r="A16" s="25">
+        <v>13</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="15">
+        <v>2</v>
+      </c>
+      <c r="D16" s="15">
+        <v>3</v>
+      </c>
+      <c r="E16" s="15">
+        <v>4</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="26"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
+      <c r="A17" s="25">
+        <v>14</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="15">
+        <v>6</v>
+      </c>
+      <c r="D17" s="15">
+        <v>9</v>
+      </c>
+      <c r="E17" s="15">
+        <v>11</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="26"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
+      <c r="A18" s="25">
+        <v>15</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="15">
+        <v>2</v>
+      </c>
+      <c r="D18" s="15">
+        <v>3</v>
+      </c>
+      <c r="E18" s="15">
+        <v>4</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="26"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="A19" s="25">
+        <v>16</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="15">
+        <v>1</v>
+      </c>
+      <c r="D19" s="15">
+        <v>3</v>
+      </c>
+      <c r="E19" s="15">
+        <v>4</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="26"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="A20" s="25">
+        <v>17</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="15">
+        <v>2</v>
+      </c>
+      <c r="D20" s="15">
+        <v>3</v>
+      </c>
+      <c r="E20" s="15">
+        <v>5</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="26"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="A21" s="25">
+        <v>18</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="15">
+        <v>3</v>
+      </c>
+      <c r="D21" s="15">
+        <v>4</v>
+      </c>
+      <c r="E21" s="15">
+        <v>5</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="26"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="A22" s="25">
+        <v>19</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="15">
+        <v>3</v>
+      </c>
+      <c r="D22" s="15">
+        <v>4</v>
+      </c>
+      <c r="E22" s="15">
+        <v>7</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="26"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="A23" s="25">
+        <v>20</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="15">
+        <v>6</v>
+      </c>
+      <c r="D23" s="15">
+        <v>10</v>
+      </c>
+      <c r="E23" s="15">
+        <v>13</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="26"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="A24" s="25">
+        <v>21</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="15">
+        <v>1</v>
+      </c>
+      <c r="D24" s="15">
+        <v>1</v>
+      </c>
+      <c r="E24" s="15">
+        <v>1</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="26"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
+      <c r="A25" s="25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="15">
+        <v>2</v>
+      </c>
+      <c r="D25" s="15">
+        <v>3</v>
+      </c>
+      <c r="E25" s="15">
+        <v>4</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="26"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="A26" s="25">
+        <v>23</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="15">
+        <v>5</v>
+      </c>
+      <c r="D26" s="15">
+        <v>7</v>
+      </c>
+      <c r="E26" s="15">
+        <v>10</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="15"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="26"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
+      <c r="A27" s="25">
+        <v>24</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="15">
+        <v>6</v>
+      </c>
+      <c r="D27" s="15">
+        <v>9</v>
+      </c>
+      <c r="E27" s="15">
+        <v>11</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="26"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="A28" s="25">
+        <v>25</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="15">
+        <v>6</v>
+      </c>
+      <c r="D28" s="15">
+        <v>10</v>
+      </c>
+      <c r="E28" s="15">
+        <v>13</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="26"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="A29" s="25">
+        <v>26</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="15">
+        <v>1</v>
+      </c>
+      <c r="D29" s="15">
+        <v>1</v>
+      </c>
+      <c r="E29" s="15">
+        <v>2</v>
+      </c>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="26"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="26"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="26"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="26"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="24"/>
-      <c r="B34" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="12"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="24"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="12"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="23"/>
-      <c r="B36" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="16">
-        <v>4</v>
-      </c>
-      <c r="D36" s="16">
-        <v>5</v>
-      </c>
-      <c r="E36" s="16">
-        <v>7</v>
-      </c>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A36" s="25"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="23"/>
-      <c r="B37" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="16">
-        <v>2</v>
-      </c>
-      <c r="D37" s="16">
-        <v>4</v>
-      </c>
-      <c r="E37" s="16">
-        <v>5</v>
-      </c>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A37" s="25"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="23"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="23"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="23"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="23"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="23"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="23"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="23"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="23"/>
-      <c r="B45" s="15"/>
+      <c r="B45" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="C45" s="16"/>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
       <c r="G45" s="16"/>
       <c r="H45" s="16"/>
+      <c r="I45" s="12"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="23"/>
-      <c r="B46" s="15"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
       <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="12"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A47" s="23"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
+      <c r="A47" s="22">
+        <v>1</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="15">
+        <v>4</v>
+      </c>
+      <c r="D47" s="15">
+        <v>5</v>
+      </c>
+      <c r="E47" s="15">
+        <v>7</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" s="23"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
+      <c r="A48" s="22">
+        <v>2</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="15">
+        <v>2</v>
+      </c>
+      <c r="D48" s="15">
+        <v>4</v>
+      </c>
+      <c r="E48" s="15">
+        <v>5</v>
+      </c>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" s="23"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
+      <c r="A49" s="22">
+        <v>3</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="15">
+        <v>3</v>
+      </c>
+      <c r="D49" s="15">
+        <v>5</v>
+      </c>
+      <c r="E49" s="15">
+        <v>7</v>
+      </c>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H49" s="15"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" s="23"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
+      <c r="A50" s="22">
+        <v>4</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="15">
+        <v>2</v>
+      </c>
+      <c r="D50" s="15">
+        <v>3</v>
+      </c>
+      <c r="E50" s="15">
+        <v>4</v>
+      </c>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" s="23"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-    </row>
-    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="25"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="19">
-        <f>SUM(C4:C51)</f>
-        <v>20</v>
-      </c>
-      <c r="D52" s="20">
-        <f>SUM(D4:D51)</f>
+      <c r="A51" s="22">
+        <v>5</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="15">
+        <v>3</v>
+      </c>
+      <c r="D51" s="15">
+        <v>5</v>
+      </c>
+      <c r="E51" s="15">
+        <v>6</v>
+      </c>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="22">
+        <v>6</v>
+      </c>
+      <c r="B52" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E52" s="21">
-        <f>SUM(E4:E51)</f>
-        <v>45</v>
-      </c>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="8"/>
+      <c r="C52" s="15">
+        <v>3</v>
+      </c>
+      <c r="D52" s="15">
+        <v>5</v>
+      </c>
+      <c r="E52" s="15">
+        <v>6</v>
+      </c>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="22">
+        <v>7</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="15">
+        <v>1</v>
+      </c>
+      <c r="D53" s="15">
+        <v>1</v>
+      </c>
+      <c r="E53" s="15">
+        <v>1</v>
+      </c>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" s="22"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B55" s="9"/>
+      <c r="A55" s="22"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B56" s="9"/>
+      <c r="A56" s="22"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B57" s="9"/>
+      <c r="A57" s="22"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B58" s="9"/>
+      <c r="A58" s="22"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" s="22"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" s="22"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" s="22"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="22"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+    </row>
+    <row r="63" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="24"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="18">
+        <f>SUM(C4:C62)</f>
+        <v>102</v>
+      </c>
+      <c r="D63" s="19">
+        <f>SUM(D4:D62)</f>
+        <v>156</v>
+      </c>
+      <c r="E63" s="20">
+        <f>SUM(E4:E62)</f>
+        <v>212</v>
+      </c>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="8"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" s="9"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B67" s="9"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B68" s="9"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B69" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F2:H2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F1:H3 F36:H1048576 F6:H6 F10:H33 F7 H7">
-    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text=":)">
+  <conditionalFormatting sqref="F1:H3 F47:H48 F6:H6 F22:H22 F7 H7 F24:H25 F50:H50 F49 F52:H1048576 F51 F26:F28 H49:H53 H22:H27 F21:G21 F23 H18:H20 G17:G20 F28:H44">
+    <cfRule type="containsText" dxfId="68" priority="88" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="67" priority="89" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="66" priority="90" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F5 H4:H5">
-    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="65" priority="85" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="26" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="64" priority="86" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="27" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="63" priority="87" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:E1048576 C10:E33 C1:E7">
-    <cfRule type="colorScale" priority="24">
+  <conditionalFormatting sqref="C47:E1048576 C22:E44 C1:E7">
+    <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="num" val="8"/>
         <cfvo type="num" val="40"/>
@@ -1554,19 +2506,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34:H35">
-    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",F34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",F34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="23" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",F34)))</formula>
+  <conditionalFormatting sqref="F45:H46">
+    <cfRule type="containsText" dxfId="62" priority="81" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",F45)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="82" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",F45)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="83" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",F45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34:E35">
-    <cfRule type="colorScale" priority="20">
+  <conditionalFormatting sqref="C45:E46">
+    <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="num" val="8"/>
         <cfvo type="num" val="40"/>
@@ -1576,58 +2528,223 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="59" priority="73" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="58" priority="74" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="57" priority="75" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="56" priority="70" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",G5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="55" priority="71" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",G5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="54" priority="72" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",G5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",H36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",H36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",H36)))</formula>
+  <conditionalFormatting sqref="H47">
+    <cfRule type="containsText" dxfId="53" priority="67" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="68" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="69" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",H37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",H37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",H37)))</formula>
+  <conditionalFormatting sqref="H48">
+    <cfRule type="containsText" dxfId="50" priority="64" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="65" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="66" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
+    <cfRule type="containsText" dxfId="47" priority="61" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="62" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="63" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G10">
+    <cfRule type="containsText" dxfId="44" priority="58" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="59" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="60" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G16">
+    <cfRule type="containsText" dxfId="41" priority="55" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="56" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="57" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H51">
+    <cfRule type="containsText" dxfId="38" priority="22" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="23" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="24" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:H10">
+    <cfRule type="containsText" dxfId="35" priority="46" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="47" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="48" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:H16">
+    <cfRule type="containsText" dxfId="32" priority="43" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="44" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="45" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="containsText" dxfId="29" priority="40" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="41" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="42" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G49">
+    <cfRule type="containsText" dxfId="26" priority="37" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="38" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="39" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H50">
+    <cfRule type="containsText" dxfId="23" priority="34" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="35" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="36" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27">
+    <cfRule type="containsText" dxfId="20" priority="31" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="32" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="33" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26">
+    <cfRule type="containsText" dxfId="17" priority="28" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="29" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="30" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G51">
+    <cfRule type="containsText" dxfId="14" priority="25" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="26" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="27" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H53)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H53)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H52">
+    <cfRule type="containsText" dxfId="8" priority="19" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="20" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="21" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H52)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H14">
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="11" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",G7)))</formula>
+      <formula>NOT(ISERROR(SEARCH(":)",G21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",G7)))</formula>
+      <formula>NOT(ISERROR(SEARCH(":|",G21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",G7)))</formula>
+      <formula>NOT(ISERROR(SEARCH(":(",G21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adicionado as views de cupom. Adicionado mais estimativas para o projeto; Arrumado a Index; Adicionado a página registration; Arrumado a Index;
</commit_message>
<xml_diff>
--- a/artefatos/ESTIMATIVA.xlsx
+++ b/artefatos/ESTIMATIVA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Laboratorio de Engenharia\Segunda tentativa\ToCBooks\artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F3B9CC-688A-4724-9064-BB13A39E6A8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECE7510-FB8E-4134-A936-700E6DC62182}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4390" yWindow="2540" windowWidth="29700" windowHeight="14020" xr2:uid="{D9FF7230-91BA-A544-8A5A-3054F2DD43A9}"/>
+    <workbookView xWindow="28460" yWindow="9580" windowWidth="29700" windowHeight="14020" xr2:uid="{D9FF7230-91BA-A544-8A5A-3054F2DD43A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
   <si>
     <t>(horas)</t>
   </si>
@@ -116,21 +116,12 @@
     <t>Criar os validadores de compra</t>
   </si>
   <si>
-    <t>Criar a lógica de compra</t>
-  </si>
-  <si>
     <t>Criar a tela de compra</t>
   </si>
   <si>
     <t>Criar a tela de devolução</t>
   </si>
   <si>
-    <t>Criar a lógica de devolução</t>
-  </si>
-  <si>
-    <t>Criar a lógica do cupom de desconto</t>
-  </si>
-  <si>
     <t>Adicionar a tela o cupom de desconto</t>
   </si>
   <si>
@@ -168,6 +159,75 @@
   </si>
   <si>
     <t>Criar classe de modelo que represente o Cartão de Crédito</t>
+  </si>
+  <si>
+    <t>Criar classe de Cartao de Crédito</t>
+  </si>
+  <si>
+    <t>Criar classe de Endereco de Cobrança</t>
+  </si>
+  <si>
+    <t>Criar classe de Endereco de Entrega</t>
+  </si>
+  <si>
+    <t>Criar classe de validador de senha forte cliente</t>
+  </si>
+  <si>
+    <t>Criar classe de Estoque</t>
+  </si>
+  <si>
+    <t>Criar classe de validador de valor de venda</t>
+  </si>
+  <si>
+    <t>Criar classe de baixa de estoque</t>
+  </si>
+  <si>
+    <t>Criar classe de validador de compra de livro</t>
+  </si>
+  <si>
+    <t>Criar a classe de devolução</t>
+  </si>
+  <si>
+    <t>Criar classe cupom de desconto</t>
+  </si>
+  <si>
+    <t>Criar validador de cliente</t>
+  </si>
+  <si>
+    <t>Criar classe validador de cartão de crédito</t>
+  </si>
+  <si>
+    <t>Criar classe validador de estoque</t>
+  </si>
+  <si>
+    <t>Criar tela de cadastro de Cliente</t>
+  </si>
+  <si>
+    <t>Criar tela de login de Cliente</t>
+  </si>
+  <si>
+    <t>Criar tela de cadastro de Livro</t>
+  </si>
+  <si>
+    <t>Criar tela de edição de Cliente</t>
+  </si>
+  <si>
+    <t>Criar tela de edição de Livro</t>
+  </si>
+  <si>
+    <t>Criar tela de Estoque</t>
+  </si>
+  <si>
+    <t>Criar tela de Listagem de Produtos</t>
+  </si>
+  <si>
+    <t>Criar tela de Página de Único produto</t>
+  </si>
+  <si>
+    <t>Criar tela do Painel Administrativo</t>
+  </si>
+  <si>
+    <t>Criar tela de alteração de Endereço de Cliente</t>
   </si>
 </sst>
 </file>
@@ -245,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -279,11 +339,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -363,11 +436,437 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="111">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1374,16 +1873,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B692412-8401-4F44-8DDD-33476696CC96}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.4140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="49.25" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="11.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="3" style="1" customWidth="1"/>
     <col min="7" max="7" width="2.83203125" style="1" customWidth="1"/>
@@ -1586,7 +2085,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10" s="15">
         <v>2</v>
@@ -1608,7 +2107,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11" s="15">
         <v>6</v>
@@ -1630,7 +2129,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" s="15">
         <v>2</v>
@@ -1652,7 +2151,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" s="15">
         <v>1</v>
@@ -1674,7 +2173,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" s="15">
         <v>2</v>
@@ -1717,7 +2216,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" s="15">
         <v>2</v>
@@ -1739,7 +2238,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C17" s="15">
         <v>6</v>
@@ -1761,7 +2260,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" s="15">
         <v>2</v>
@@ -1783,7 +2282,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19" s="15">
         <v>1</v>
@@ -1805,7 +2304,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C20" s="15">
         <v>2</v>
@@ -1849,7 +2348,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C22" s="15">
         <v>3</v>
@@ -1915,16 +2414,16 @@
         <v>22</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C25" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E25" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
@@ -1937,65 +2436,65 @@
         <v>23</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C26" s="15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D26" s="15">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E26" s="15">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F26" s="15"/>
-      <c r="G26" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="25">
         <v>24</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C27" s="15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D27" s="15">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E27" s="15">
-        <v>11</v>
-      </c>
-      <c r="F27" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="F27" s="15"/>
       <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
+      <c r="H27" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="25">
         <v>25</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C28" s="15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D28" s="15">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E28" s="15">
-        <v>13</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -2003,7 +2502,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C29" s="15">
         <v>1</v>
@@ -2012,7 +2511,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -2021,107 +2520,229 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="25"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
+      <c r="A30" s="25">
+        <v>27</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="15">
+        <v>4</v>
+      </c>
+      <c r="D30" s="15">
+        <v>5</v>
+      </c>
+      <c r="E30" s="15">
+        <v>7</v>
+      </c>
       <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
+      <c r="G30" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="25"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
+      <c r="A31" s="25">
+        <v>28</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="15">
+        <v>3</v>
+      </c>
+      <c r="D31" s="15">
+        <v>5</v>
+      </c>
+      <c r="E31" s="15">
+        <v>7</v>
+      </c>
       <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
+      <c r="G31" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="25"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
+      <c r="A32" s="25">
+        <v>29</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="15">
+        <v>2</v>
+      </c>
+      <c r="D32" s="15">
+        <v>3</v>
+      </c>
+      <c r="E32" s="15">
+        <v>4</v>
+      </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="25"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
+      <c r="H32" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="25">
+        <v>30</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="15">
+        <v>5</v>
+      </c>
+      <c r="D33" s="15">
+        <v>7</v>
+      </c>
+      <c r="E33" s="15">
+        <v>10</v>
+      </c>
       <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
+      <c r="G33" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="25"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="25">
+        <v>31</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="15">
+        <v>3</v>
+      </c>
+      <c r="D34" s="15">
+        <v>6</v>
+      </c>
+      <c r="E34" s="15">
+        <v>9</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="25"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="25">
+        <v>32</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="15">
+        <v>6</v>
+      </c>
+      <c r="D35" s="15">
+        <v>9</v>
+      </c>
+      <c r="E35" s="15">
+        <v>11</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="25"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="25">
+        <v>33</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="15">
+        <v>6</v>
+      </c>
+      <c r="D36" s="15">
+        <v>10</v>
+      </c>
+      <c r="E36" s="15">
+        <v>13</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="25"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="25">
+        <v>34</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="15">
+        <v>1</v>
+      </c>
+      <c r="D37" s="15">
+        <v>1</v>
+      </c>
+      <c r="E37" s="15">
+        <v>2</v>
+      </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="25"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
+      <c r="H37" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="25">
+        <v>35</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="15">
+        <v>2</v>
+      </c>
+      <c r="D38" s="15">
+        <v>3</v>
+      </c>
+      <c r="E38" s="15">
+        <v>4</v>
+      </c>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="25"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
+      <c r="H38" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="25">
+        <v>36</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="15">
+        <v>4</v>
+      </c>
+      <c r="D39" s="15">
+        <v>5</v>
+      </c>
+      <c r="E39" s="15">
+        <v>7</v>
+      </c>
       <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
+      <c r="G39" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="H39" s="15"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="25"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="25">
+        <v>37</v>
+      </c>
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
@@ -2130,8 +2751,10 @@
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="25"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="25">
+        <v>38</v>
+      </c>
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
@@ -2140,8 +2763,10 @@
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="25"/>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="25">
+        <v>39</v>
+      </c>
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
       <c r="D42" s="15"/>
@@ -2150,8 +2775,10 @@
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="25"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="25">
+        <v>40</v>
+      </c>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
@@ -2160,8 +2787,10 @@
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="25"/>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="25">
+        <v>41</v>
+      </c>
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
@@ -2170,334 +2799,644 @@
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="23"/>
-      <c r="B45" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="12"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="23"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="12"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A47" s="22">
-        <v>1</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="15">
-        <v>4</v>
-      </c>
-      <c r="D47" s="15">
-        <v>5</v>
-      </c>
-      <c r="E47" s="15">
-        <v>7</v>
-      </c>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="25">
+        <v>42</v>
+      </c>
+      <c r="B45" s="14"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="25">
+        <v>43</v>
+      </c>
+      <c r="B46" s="14"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="25">
+        <v>44</v>
+      </c>
+      <c r="B47" s="14"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
-      <c r="H47" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" s="22">
-        <v>2</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="15">
-        <v>2</v>
-      </c>
-      <c r="D48" s="15">
-        <v>4</v>
-      </c>
-      <c r="E48" s="15">
-        <v>5</v>
-      </c>
+      <c r="H47" s="15"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="25">
+        <v>45</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
       <c r="F48" s="15"/>
       <c r="G48" s="15"/>
-      <c r="H48" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="H48" s="15"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" s="22">
-        <v>3</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" s="15">
-        <v>3</v>
-      </c>
-      <c r="D49" s="15">
-        <v>5</v>
-      </c>
-      <c r="E49" s="15">
-        <v>7</v>
-      </c>
+      <c r="A49" s="25">
+        <v>46</v>
+      </c>
+      <c r="B49" s="14"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
       <c r="F49" s="15"/>
-      <c r="G49" s="15" t="s">
-        <v>2</v>
-      </c>
+      <c r="G49" s="15"/>
       <c r="H49" s="15"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" s="22">
-        <v>4</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" s="15">
-        <v>2</v>
-      </c>
-      <c r="D50" s="15">
-        <v>3</v>
-      </c>
-      <c r="E50" s="15">
-        <v>4</v>
-      </c>
+      <c r="A50" s="25">
+        <v>47</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
       <c r="F50" s="15"/>
       <c r="G50" s="15"/>
-      <c r="H50" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="H50" s="15"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" s="22">
-        <v>5</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C51" s="15">
-        <v>3</v>
-      </c>
-      <c r="D51" s="15">
-        <v>5</v>
-      </c>
-      <c r="E51" s="15">
-        <v>6</v>
-      </c>
+      <c r="A51" s="25">
+        <v>48</v>
+      </c>
+      <c r="B51" s="14"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
       <c r="F51" s="15"/>
       <c r="G51" s="15"/>
-      <c r="H51" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="H51" s="15"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" s="22">
-        <v>6</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C52" s="15">
-        <v>3</v>
-      </c>
-      <c r="D52" s="15">
-        <v>5</v>
-      </c>
-      <c r="E52" s="15">
-        <v>6</v>
-      </c>
+      <c r="A52" s="25">
+        <v>49</v>
+      </c>
+      <c r="B52" s="14"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
       <c r="F52" s="15"/>
       <c r="G52" s="15"/>
-      <c r="H52" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="H52" s="15"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="22">
+      <c r="A53" s="23"/>
+      <c r="B53" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="12"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" s="27"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="12"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" s="22">
+        <v>1</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="15">
+        <v>4</v>
+      </c>
+      <c r="D55" s="15">
+        <v>5</v>
+      </c>
+      <c r="E55" s="15">
         <v>7</v>
       </c>
-      <c r="B53" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="15">
-        <v>1</v>
-      </c>
-      <c r="D53" s="15">
-        <v>1</v>
-      </c>
-      <c r="E53" s="15">
-        <v>1</v>
-      </c>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="22"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" s="22"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
       <c r="F55" s="15"/>
       <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
+      <c r="H55" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" s="22"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
+      <c r="A56" s="22">
+        <v>2</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="15">
+        <v>2</v>
+      </c>
+      <c r="D56" s="15">
+        <v>4</v>
+      </c>
+      <c r="E56" s="15">
+        <v>5</v>
+      </c>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
-      <c r="H56" s="15"/>
+      <c r="H56" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" s="22"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
+      <c r="A57" s="22">
+        <v>3</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="15">
+        <v>3</v>
+      </c>
+      <c r="D57" s="15">
+        <v>5</v>
+      </c>
+      <c r="E57" s="15">
+        <v>7</v>
+      </c>
       <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
+      <c r="G57" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="H57" s="15"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" s="22"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
+      <c r="A58" s="22">
+        <v>4</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="15">
+        <v>2</v>
+      </c>
+      <c r="D58" s="15">
+        <v>3</v>
+      </c>
+      <c r="E58" s="15">
+        <v>4</v>
+      </c>
       <c r="F58" s="15"/>
       <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
+      <c r="H58" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59" s="22"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
+      <c r="A59" s="22">
+        <v>5</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="15">
+        <v>3</v>
+      </c>
+      <c r="D59" s="15">
+        <v>5</v>
+      </c>
+      <c r="E59" s="15">
+        <v>6</v>
+      </c>
       <c r="F59" s="15"/>
       <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
+      <c r="H59" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60" s="22"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
+      <c r="A60" s="22">
+        <v>6</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" s="15">
+        <v>3</v>
+      </c>
+      <c r="D60" s="15">
+        <v>5</v>
+      </c>
+      <c r="E60" s="15">
+        <v>6</v>
+      </c>
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
+      <c r="H60" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" s="22"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
+      <c r="A61" s="22">
+        <v>7</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61" s="15">
+        <v>1</v>
+      </c>
+      <c r="D61" s="15">
+        <v>1</v>
+      </c>
+      <c r="E61" s="15">
+        <v>1</v>
+      </c>
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
-      <c r="H61" s="15"/>
+      <c r="H61" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" s="22"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
+      <c r="A62" s="22">
+        <v>8</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="15">
+        <v>3</v>
+      </c>
+      <c r="D62" s="15">
+        <v>5</v>
+      </c>
+      <c r="E62" s="15">
+        <v>6</v>
+      </c>
       <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
+      <c r="G62" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="H62" s="15"/>
     </row>
-    <row r="63" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="24"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18">
-        <f>SUM(C4:C62)</f>
-        <v>102</v>
-      </c>
-      <c r="D63" s="19">
-        <f>SUM(D4:D62)</f>
-        <v>156</v>
-      </c>
-      <c r="E63" s="20">
-        <f>SUM(E4:E62)</f>
-        <v>212</v>
-      </c>
-      <c r="F63" s="21"/>
-      <c r="G63" s="21"/>
-      <c r="H63" s="21"/>
-      <c r="I63" s="8"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" s="9"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" s="9"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B68" s="9"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B69" s="9"/>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="22">
+        <v>9</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="15">
+        <v>3</v>
+      </c>
+      <c r="D63" s="15">
+        <v>5</v>
+      </c>
+      <c r="E63" s="15">
+        <v>6</v>
+      </c>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" s="22">
+        <v>10</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C64" s="15">
+        <v>2</v>
+      </c>
+      <c r="D64" s="15">
+        <v>4</v>
+      </c>
+      <c r="E64" s="15">
+        <v>6</v>
+      </c>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H64" s="15"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" s="22">
+        <v>11</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C65" s="15">
+        <v>4</v>
+      </c>
+      <c r="D65" s="15">
+        <v>6</v>
+      </c>
+      <c r="E65" s="15">
+        <v>10</v>
+      </c>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H65" s="15"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" s="22">
+        <v>12</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" s="15">
+        <v>4</v>
+      </c>
+      <c r="D66" s="15">
+        <v>5</v>
+      </c>
+      <c r="E66" s="15">
+        <v>8</v>
+      </c>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H66" s="15"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" s="22">
+        <v>13</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C67" s="15">
+        <v>5</v>
+      </c>
+      <c r="D67" s="15">
+        <v>8</v>
+      </c>
+      <c r="E67" s="15">
+        <v>11</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" s="22">
+        <v>14</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" s="15">
+        <v>4</v>
+      </c>
+      <c r="D68" s="15">
+        <v>5</v>
+      </c>
+      <c r="E68" s="15">
+        <v>10</v>
+      </c>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H68" s="15"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" s="22">
+        <v>15</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C69" s="15">
+        <v>3</v>
+      </c>
+      <c r="D69" s="15">
+        <v>5</v>
+      </c>
+      <c r="E69" s="15">
+        <v>6</v>
+      </c>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H69" s="15"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" s="22">
+        <v>16</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C70" s="15">
+        <v>5</v>
+      </c>
+      <c r="D70" s="15">
+        <v>6</v>
+      </c>
+      <c r="E70" s="15">
+        <v>7</v>
+      </c>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H70" s="15"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" s="22">
+        <v>17</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" s="15">
+        <v>3</v>
+      </c>
+      <c r="D71" s="15">
+        <v>5</v>
+      </c>
+      <c r="E71" s="15">
+        <v>7</v>
+      </c>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A72" s="22">
+        <v>18</v>
+      </c>
+      <c r="B72" s="14"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" s="22">
+        <v>19</v>
+      </c>
+      <c r="B73" s="14"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" s="22">
+        <v>20</v>
+      </c>
+      <c r="B74" s="14"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" s="22">
+        <v>21</v>
+      </c>
+      <c r="B75" s="14"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76" s="22">
+        <v>22</v>
+      </c>
+      <c r="B76" s="14"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" s="22">
+        <v>23</v>
+      </c>
+      <c r="B77" s="14"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" s="22">
+        <v>24</v>
+      </c>
+      <c r="B78" s="14"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+    </row>
+    <row r="79" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="24"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="18">
+        <f>SUM(C4:C78)</f>
+        <v>160</v>
+      </c>
+      <c r="D79" s="19">
+        <f>SUM(D4:D78)</f>
+        <v>240</v>
+      </c>
+      <c r="E79" s="20">
+        <f>SUM(E4:E78)</f>
+        <v>331</v>
+      </c>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
+      <c r="H79" s="21"/>
+      <c r="I79" s="8"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B82" s="9"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B83" s="9"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B84" s="9"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B85" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F2:H2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F1:H3 F47:H48 F6:H6 F22:H22 F7 H7 F24:H25 F50:H50 F49 F52:H1048576 F51 F26:F28 H49:H53 H22:H27 F21:G21 F23 H18:H20 G17:G20 F28:H44">
-    <cfRule type="containsText" dxfId="68" priority="88" operator="containsText" text=":)">
+  <conditionalFormatting sqref="F1:H3 F55:H56 F6:H6 F22:H22 F7 H7 F24:H27 F58:H58 F57 F60:H61 F59 F21:G21 F23 H18:H20 G17:G20 F32:H32 F29:H29 F28 F30:F31 H22:H35 F33:F36 F36:H38 F40:H52 F39 H39 F63:H63 F62 F67:H67 H57:H66 F71:H1048576 F64:F70 H68:H71">
+    <cfRule type="containsText" dxfId="110" priority="133" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="89" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="109" priority="134" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="90" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="108" priority="135" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F5 H4:H5">
-    <cfRule type="containsText" dxfId="65" priority="85" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="107" priority="130" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="86" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="106" priority="131" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="87" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="105" priority="132" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47:E1048576 C22:E44 C1:E7">
-    <cfRule type="colorScale" priority="84">
+  <conditionalFormatting sqref="C22:E52 C1:E7 C55:E1048576">
+    <cfRule type="colorScale" priority="129">
       <colorScale>
         <cfvo type="num" val="8"/>
         <cfvo type="num" val="40"/>
@@ -2506,19 +3445,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45:H46">
-    <cfRule type="containsText" dxfId="62" priority="81" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",F45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="82" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",F45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="83" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",F45)))</formula>
+  <conditionalFormatting sqref="F53:H54">
+    <cfRule type="containsText" dxfId="104" priority="126" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",F53)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="127" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",F53)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="128" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",F53)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45:E46">
-    <cfRule type="colorScale" priority="80">
+  <conditionalFormatting sqref="C53:E54">
+    <cfRule type="colorScale" priority="125">
       <colorScale>
         <cfvo type="num" val="8"/>
         <cfvo type="num" val="40"/>
@@ -2528,223 +3467,377 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="containsText" dxfId="59" priority="73" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="101" priority="118" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="74" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="100" priority="119" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="75" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="99" priority="120" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="56" priority="70" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="98" priority="115" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",G5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="71" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="97" priority="116" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",G5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="72" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="96" priority="117" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",G5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
-    <cfRule type="containsText" dxfId="53" priority="67" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",H47)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="68" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",H47)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="69" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",H47)))</formula>
+  <conditionalFormatting sqref="H55">
+    <cfRule type="containsText" dxfId="95" priority="112" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H55)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="113" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H55)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="93" priority="114" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H55)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
-    <cfRule type="containsText" dxfId="50" priority="64" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",H48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="65" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",H48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="66" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",H48)))</formula>
+  <conditionalFormatting sqref="H56">
+    <cfRule type="containsText" dxfId="92" priority="109" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="91" priority="110" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="111" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="containsText" dxfId="47" priority="61" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="89" priority="106" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",G7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="62" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="88" priority="107" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",G7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="63" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="87" priority="108" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",G7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G10">
-    <cfRule type="containsText" dxfId="44" priority="58" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="86" priority="103" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="59" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="85" priority="104" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="60" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="84" priority="105" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G16">
-    <cfRule type="containsText" dxfId="41" priority="55" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="83" priority="100" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",G11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="56" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="82" priority="101" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",G11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="57" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="81" priority="102" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
-    <cfRule type="containsText" dxfId="38" priority="22" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",H51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="23" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",H51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="24" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",H51)))</formula>
+  <conditionalFormatting sqref="H59">
+    <cfRule type="containsText" dxfId="80" priority="67" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H59)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="79" priority="68" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H59)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="69" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H10">
-    <cfRule type="containsText" dxfId="35" priority="46" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="77" priority="91" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="47" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="76" priority="92" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="48" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="75" priority="93" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:H16">
-    <cfRule type="containsText" dxfId="32" priority="43" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="74" priority="88" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",H15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="44" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="73" priority="89" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",H15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="45" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="72" priority="90" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",H15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="containsText" dxfId="29" priority="40" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="71" priority="85" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",G23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="41" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="70" priority="86" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",G23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="42" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="69" priority="87" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",G23)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="26" priority="37" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",G49)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="38" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",G49)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="39" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",G49)))</formula>
+  <conditionalFormatting sqref="G57">
+    <cfRule type="containsText" dxfId="68" priority="82" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G57)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="83" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G57)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="84" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G57)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="containsText" dxfId="23" priority="34" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",H50)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="35" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",H50)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="36" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",H50)))</formula>
+  <conditionalFormatting sqref="H58">
+    <cfRule type="containsText" dxfId="65" priority="79" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="80" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="81" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H58)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G27">
-    <cfRule type="containsText" dxfId="20" priority="31" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",G27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="32" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",G27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="33" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",G27)))</formula>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="containsText" dxfId="62" priority="76" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="77" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="78" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G35)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26">
-    <cfRule type="containsText" dxfId="17" priority="28" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",G26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="29" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",G26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="30" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",G26)))</formula>
+  <conditionalFormatting sqref="G33:G34">
+    <cfRule type="containsText" dxfId="59" priority="73" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="74" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="75" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G33)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="14" priority="25" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",G51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="26" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",G51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="27" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",G51)))</formula>
+  <conditionalFormatting sqref="G59">
+    <cfRule type="containsText" dxfId="56" priority="70" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G59)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="71" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G59)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="72" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G59)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H53">
-    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",H53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",H53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",H53)))</formula>
+  <conditionalFormatting sqref="H61">
+    <cfRule type="containsText" dxfId="53" priority="61" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H61)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="62" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H61)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="63" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H61)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H52">
-    <cfRule type="containsText" dxfId="8" priority="19" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",H52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="20" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",H52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="21" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",H52)))</formula>
+  <conditionalFormatting sqref="H60">
+    <cfRule type="containsText" dxfId="50" priority="64" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H60)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="65" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H60)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="66" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H14">
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="47" priority="55" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",H12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="11" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="46" priority="56" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",H12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="45" priority="57" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",H12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
+    <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31">
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30">
+    <cfRule type="containsText" dxfId="35" priority="37" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="38" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39">
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G62">
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H63:H64">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G64">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G65">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G66">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G69">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G69)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G69)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G68">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H70">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",H70)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",H70)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",H70)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G70">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text=":)">
+      <formula>NOT(ISERROR(SEARCH(":)",G70)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text=":|">
+      <formula>NOT(ISERROR(SEARCH(":|",G70)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text=":(">
+      <formula>NOT(ISERROR(SEARCH(":(",G70)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H71">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",G21)))</formula>
+      <formula>NOT(ISERROR(SEARCH(":)",H71)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",G21)))</formula>
+      <formula>NOT(ISERROR(SEARCH(":|",H71)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",G21)))</formula>
+      <formula>NOT(ISERROR(SEARCH(":(",H71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2879,20 +3972,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="85d3bf16-a445-4c91-92d7-e8d893ae22c3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="85d3bf16-a445-4c91-92d7-e8d893ae22c3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2914,6 +4007,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A55BC6FF-54C9-4DD8-8203-E7CA3890AFA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C51C229-CA01-440E-B2BE-F6F69B7DA214}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2921,12 +4022,4 @@
     <ds:schemaRef ds:uri="85d3bf16-a445-4c91-92d7-e8d893ae22c3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A55BC6FF-54C9-4DD8-8203-E7CA3890AFA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>